<commit_message>
Update - Final Version
</commit_message>
<xml_diff>
--- a/Protected Sites Tracker Transfer/Assets/SSSI List.xlsx
+++ b/Protected Sites Tracker Transfer/Assets/SSSI List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/kai_lumber_defra_gov_uk/Documents/UiPath Working Folder/NE-Protected-Sites-Tracker-Transfer/Protected Sites Tracker Transfer/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{BCE4E5F5-1A98-4DCD-BBDA-6367ED51A32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{256E2253-C64F-494E-9347-67C52EEA5181}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{BCE4E5F5-1A98-4DCD-BBDA-6367ED51A32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD59DCEF-9BA4-48DD-BF9A-2E6428FC16E7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8880" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F37F3E-0F04-49DF-AE6C-9D2E59337BCF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B7F37F3E-0F04-49DF-AE6C-9D2E59337BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="SSSI List" sheetId="1" r:id="rId1"/>
@@ -2359,9 +2359,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2698,21 +2704,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51A7658-85E0-4753-AC32-483A0304837B}">
   <dimension ref="A1:B420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="A413" sqref="A413"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="62.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122.62890625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>745</v>
       </c>
     </row>
@@ -2720,7 +2726,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2728,7 +2734,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2736,7 +2742,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2744,7 +2750,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2752,7 +2758,7 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2760,7 +2766,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2768,15 +2774,15 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2784,7 +2790,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2792,7 +2798,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2800,7 +2806,7 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2808,7 +2814,7 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2816,7 +2822,7 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2824,7 +2830,7 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2832,7 +2838,7 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2840,15 +2846,15 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2856,7 +2862,7 @@
       <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2864,7 +2870,7 @@
       <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2872,7 +2878,7 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2880,7 +2886,7 @@
       <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2888,7 +2894,7 @@
       <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2896,7 +2902,7 @@
       <c r="A24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2904,7 +2910,7 @@
       <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2912,7 +2918,7 @@
       <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2920,7 +2926,7 @@
       <c r="A27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2928,15 +2934,15 @@
       <c r="A28" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2944,7 +2950,7 @@
       <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2952,7 +2958,7 @@
       <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2960,7 +2966,7 @@
       <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2968,7 +2974,7 @@
       <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2976,7 +2982,7 @@
       <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2984,7 +2990,7 @@
       <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2992,7 +2998,7 @@
       <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3000,7 +3006,7 @@
       <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3008,23 +3014,23 @@
       <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3032,7 +3038,7 @@
       <c r="A41" t="s">
         <v>77</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3040,7 +3046,7 @@
       <c r="A42" t="s">
         <v>79</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3048,7 +3054,7 @@
       <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3056,15 +3062,15 @@
       <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>85</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3072,7 +3078,7 @@
       <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3080,7 +3086,7 @@
       <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3088,15 +3094,15 @@
       <c r="A48" t="s">
         <v>91</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>93</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3104,7 +3110,7 @@
       <c r="A50" t="s">
         <v>95</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3112,7 +3118,7 @@
       <c r="A51" t="s">
         <v>97</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3120,7 +3126,7 @@
       <c r="A52" t="s">
         <v>747</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3128,7 +3134,7 @@
       <c r="A53" t="s">
         <v>100</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3136,7 +3142,7 @@
       <c r="A54" t="s">
         <v>102</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3144,39 +3150,39 @@
       <c r="A55" t="s">
         <v>104</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>106</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>108</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>110</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>112</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3184,7 +3190,7 @@
       <c r="A60" t="s">
         <v>114</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3192,15 +3198,15 @@
       <c r="A61" t="s">
         <v>116</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>118</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3208,7 +3214,7 @@
       <c r="A63" t="s">
         <v>120</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3216,7 +3222,7 @@
       <c r="A64" t="s">
         <v>122</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3224,7 +3230,7 @@
       <c r="A65" t="s">
         <v>124</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3232,7 +3238,7 @@
       <c r="A66" t="s">
         <v>756</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3240,7 +3246,7 @@
       <c r="A67" t="s">
         <v>127</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3248,7 +3254,7 @@
       <c r="A68" t="s">
         <v>129</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3256,7 +3262,7 @@
       <c r="A69" t="s">
         <v>131</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3264,7 +3270,7 @@
       <c r="A70" t="s">
         <v>133</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3272,7 +3278,7 @@
       <c r="A71" t="s">
         <v>135</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3280,7 +3286,7 @@
       <c r="A72" t="s">
         <v>137</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3288,7 +3294,7 @@
       <c r="A73" t="s">
         <v>139</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3296,7 +3302,7 @@
       <c r="A74" t="s">
         <v>141</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3304,7 +3310,7 @@
       <c r="A75" t="s">
         <v>143</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3312,7 +3318,7 @@
       <c r="A76" t="s">
         <v>144</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3320,7 +3326,7 @@
       <c r="A77" t="s">
         <v>146</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3328,7 +3334,7 @@
       <c r="A78" t="s">
         <v>148</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="3" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3336,7 +3342,7 @@
       <c r="A79" t="s">
         <v>150</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3344,7 +3350,7 @@
       <c r="A80" t="s">
         <v>152</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3352,7 +3358,7 @@
       <c r="A81" t="s">
         <v>154</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3360,7 +3366,7 @@
       <c r="A82" t="s">
         <v>156</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3368,7 +3374,7 @@
       <c r="A83" t="s">
         <v>158</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="3" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3376,7 +3382,7 @@
       <c r="A84" t="s">
         <v>160</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3384,7 +3390,7 @@
       <c r="A85" t="s">
         <v>162</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>163</v>
       </c>
     </row>
@@ -3392,7 +3398,7 @@
       <c r="A86" t="s">
         <v>164</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3400,7 +3406,7 @@
       <c r="A87" t="s">
         <v>166</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3408,15 +3414,15 @@
       <c r="A88" t="s">
         <v>168</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>170</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="3" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3424,7 +3430,7 @@
       <c r="A90" t="s">
         <v>172</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3432,7 +3438,7 @@
       <c r="A91" t="s">
         <v>174</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="3" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3440,7 +3446,7 @@
       <c r="A92" t="s">
         <v>176</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="3" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3448,23 +3454,23 @@
       <c r="A93" t="s">
         <v>178</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>180</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>182</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="3" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3472,7 +3478,7 @@
       <c r="A96" t="s">
         <v>184</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3480,15 +3486,15 @@
       <c r="A97" t="s">
         <v>186</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
         <v>188</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3496,7 +3502,7 @@
       <c r="A99" t="s">
         <v>190</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="3" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3504,7 +3510,7 @@
       <c r="A100" t="s">
         <v>192</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="3" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3512,7 +3518,7 @@
       <c r="A101" t="s">
         <v>194</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="3" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3525,7 +3531,7 @@
       <c r="A103" t="s">
         <v>196</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="3" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3533,7 +3539,7 @@
       <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3541,7 +3547,7 @@
       <c r="A105" t="s">
         <v>200</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="3" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3549,7 +3555,7 @@
       <c r="A106" t="s">
         <v>202</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="3" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3557,7 +3563,7 @@
       <c r="A107" t="s">
         <v>204</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3565,7 +3571,7 @@
       <c r="A108" t="s">
         <v>206</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="3" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3573,7 +3579,7 @@
       <c r="A109" t="s">
         <v>208</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="3" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3581,7 +3587,7 @@
       <c r="A110" t="s">
         <v>210</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="3" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3589,7 +3595,7 @@
       <c r="A111" t="s">
         <v>212</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="3" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3597,7 +3603,7 @@
       <c r="A112" t="s">
         <v>214</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="3" t="s">
         <v>215</v>
       </c>
     </row>
@@ -3605,7 +3611,7 @@
       <c r="A113" t="s">
         <v>757</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3613,15 +3619,15 @@
       <c r="A114" t="s">
         <v>217</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>219</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="3" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3629,7 +3635,7 @@
       <c r="A116" t="s">
         <v>221</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="3" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3637,7 +3643,7 @@
       <c r="A117" t="s">
         <v>223</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="3" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3645,7 +3651,7 @@
       <c r="A118" t="s">
         <v>225</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="3" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3653,7 +3659,7 @@
       <c r="A119" t="s">
         <v>227</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="3" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3661,7 +3667,7 @@
       <c r="A120" t="s">
         <v>229</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="3" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3669,15 +3675,15 @@
       <c r="A121" t="s">
         <v>231</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>233</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="3" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3685,7 +3691,7 @@
       <c r="A123" t="s">
         <v>235</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="3" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3693,7 +3699,7 @@
       <c r="A124" t="s">
         <v>237</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="3" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3701,7 +3707,7 @@
       <c r="A125" t="s">
         <v>239</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="3" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3709,7 +3715,7 @@
       <c r="A126" t="s">
         <v>753</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="3" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3717,7 +3723,7 @@
       <c r="A127" t="s">
         <v>242</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="3" t="s">
         <v>243</v>
       </c>
     </row>
@@ -3725,7 +3731,7 @@
       <c r="A128" t="s">
         <v>244</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="3" t="s">
         <v>245</v>
       </c>
     </row>
@@ -3733,7 +3739,7 @@
       <c r="A129" t="s">
         <v>246</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="3" t="s">
         <v>247</v>
       </c>
     </row>
@@ -3741,23 +3747,23 @@
       <c r="A130" t="s">
         <v>248</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>250</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>252</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="3" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3765,7 +3771,7 @@
       <c r="A133" t="s">
         <v>254</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="3" t="s">
         <v>255</v>
       </c>
     </row>
@@ -3773,7 +3779,7 @@
       <c r="A134" t="s">
         <v>256</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="3" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3781,7 +3787,7 @@
       <c r="A135" t="s">
         <v>258</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="3" t="s">
         <v>259</v>
       </c>
     </row>
@@ -3789,7 +3795,7 @@
       <c r="A136" t="s">
         <v>260</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="3" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3797,7 +3803,7 @@
       <c r="A137" t="s">
         <v>262</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="3" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3805,7 +3811,7 @@
       <c r="A138" t="s">
         <v>264</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="3" t="s">
         <v>265</v>
       </c>
     </row>
@@ -3813,7 +3819,7 @@
       <c r="A139" t="s">
         <v>266</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="3" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3821,15 +3827,15 @@
       <c r="A140" t="s">
         <v>268</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>270</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="3" t="s">
         <v>271</v>
       </c>
     </row>
@@ -3837,7 +3843,7 @@
       <c r="A142" t="s">
         <v>272</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="3" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3845,7 +3851,7 @@
       <c r="A143" t="s">
         <v>274</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="3" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3853,7 +3859,7 @@
       <c r="A144" t="s">
         <v>276</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="3" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3861,7 +3867,7 @@
       <c r="A145" t="s">
         <v>278</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="3" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3869,7 +3875,7 @@
       <c r="A146" t="s">
         <v>280</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="3" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3877,7 +3883,7 @@
       <c r="A147" t="s">
         <v>282</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="3" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3885,7 +3891,7 @@
       <c r="A148" t="s">
         <v>284</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="3" t="s">
         <v>285</v>
       </c>
     </row>
@@ -3893,7 +3899,7 @@
       <c r="A149" t="s">
         <v>286</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="3" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3901,15 +3907,15 @@
       <c r="A150" t="s">
         <v>288</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>290</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="3" t="s">
         <v>291</v>
       </c>
     </row>
@@ -3917,7 +3923,7 @@
       <c r="A152" t="s">
         <v>292</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="3" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3925,7 +3931,7 @@
       <c r="A153" t="s">
         <v>294</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="3" t="s">
         <v>295</v>
       </c>
     </row>
@@ -3933,7 +3939,7 @@
       <c r="A154" t="s">
         <v>296</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="3" t="s">
         <v>297</v>
       </c>
     </row>
@@ -3941,7 +3947,7 @@
       <c r="A155" t="s">
         <v>298</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="3" t="s">
         <v>299</v>
       </c>
     </row>
@@ -3949,7 +3955,7 @@
       <c r="A156" t="s">
         <v>300</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="3" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3957,7 +3963,7 @@
       <c r="A157" t="s">
         <v>302</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="3" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3965,7 +3971,7 @@
       <c r="A158" t="s">
         <v>304</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="3" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3973,7 +3979,7 @@
       <c r="A159" t="s">
         <v>306</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="3" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3981,7 +3987,7 @@
       <c r="A160" t="s">
         <v>308</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="3" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3989,7 +3995,7 @@
       <c r="A161" t="s">
         <v>310</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="3" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3997,7 +4003,7 @@
       <c r="A162" t="s">
         <v>312</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="3" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4005,7 +4011,7 @@
       <c r="A163" t="s">
         <v>314</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="3" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4013,7 +4019,7 @@
       <c r="A164" t="s">
         <v>316</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="3" t="s">
         <v>317</v>
       </c>
     </row>
@@ -4026,7 +4032,7 @@
       <c r="A166" t="s">
         <v>319</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4034,7 +4040,7 @@
       <c r="A167" t="s">
         <v>320</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="3" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4042,7 +4048,7 @@
       <c r="A168" t="s">
         <v>322</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="3" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4050,7 +4056,7 @@
       <c r="A169" t="s">
         <v>324</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="3" t="s">
         <v>325</v>
       </c>
     </row>
@@ -4058,7 +4064,7 @@
       <c r="A170" t="s">
         <v>326</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="3" t="s">
         <v>327</v>
       </c>
     </row>
@@ -4066,7 +4072,7 @@
       <c r="A171" t="s">
         <v>328</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="3" t="s">
         <v>329</v>
       </c>
     </row>
@@ -4074,7 +4080,7 @@
       <c r="A172" t="s">
         <v>330</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="3" t="s">
         <v>331</v>
       </c>
     </row>
@@ -4082,7 +4088,7 @@
       <c r="A173" t="s">
         <v>332</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B173" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4090,7 +4096,7 @@
       <c r="A174" t="s">
         <v>334</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="3" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4098,7 +4104,7 @@
       <c r="A175" t="s">
         <v>336</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="3" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4106,7 +4112,7 @@
       <c r="A176" t="s">
         <v>338</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="3" t="s">
         <v>339</v>
       </c>
     </row>
@@ -4119,7 +4125,7 @@
       <c r="A178" t="s">
         <v>341</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="3" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4127,15 +4133,15 @@
       <c r="A179" t="s">
         <v>343</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="3" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>345</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="3" t="s">
         <v>346</v>
       </c>
     </row>
@@ -4143,7 +4149,7 @@
       <c r="A181" t="s">
         <v>347</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="3" t="s">
         <v>348</v>
       </c>
     </row>
@@ -4151,7 +4157,7 @@
       <c r="A182" t="s">
         <v>349</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="3" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4159,7 +4165,7 @@
       <c r="A183" t="s">
         <v>351</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="3" t="s">
         <v>352</v>
       </c>
     </row>
@@ -4167,15 +4173,15 @@
       <c r="A184" t="s">
         <v>353</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="3" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>355</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="3" t="s">
         <v>356</v>
       </c>
     </row>
@@ -4188,7 +4194,7 @@
       <c r="A187" t="s">
         <v>358</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="3" t="s">
         <v>359</v>
       </c>
     </row>
@@ -4196,7 +4202,7 @@
       <c r="A188" t="s">
         <v>360</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="3" t="s">
         <v>361</v>
       </c>
     </row>
@@ -4209,7 +4215,7 @@
       <c r="A190" t="s">
         <v>363</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="3" t="s">
         <v>364</v>
       </c>
     </row>
@@ -4217,7 +4223,7 @@
       <c r="A191" t="s">
         <v>365</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4225,7 +4231,7 @@
       <c r="A192" t="s">
         <v>366</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="3" t="s">
         <v>367</v>
       </c>
     </row>
@@ -4233,7 +4239,7 @@
       <c r="A193" t="s">
         <v>368</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="3" t="s">
         <v>369</v>
       </c>
     </row>
@@ -4246,7 +4252,7 @@
       <c r="A195" t="s">
         <v>371</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="3" t="s">
         <v>372</v>
       </c>
     </row>
@@ -4254,7 +4260,7 @@
       <c r="A196" t="s">
         <v>373</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="3" t="s">
         <v>374</v>
       </c>
     </row>
@@ -4267,7 +4273,7 @@
       <c r="A198" t="s">
         <v>376</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="3" t="s">
         <v>377</v>
       </c>
     </row>
@@ -4275,7 +4281,7 @@
       <c r="A199" t="s">
         <v>378</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="3" t="s">
         <v>379</v>
       </c>
     </row>
@@ -4283,7 +4289,7 @@
       <c r="A200" t="s">
         <v>380</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="3" t="s">
         <v>381</v>
       </c>
     </row>
@@ -4291,7 +4297,7 @@
       <c r="A201" t="s">
         <v>382</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -4299,7 +4305,7 @@
       <c r="A202" t="s">
         <v>383</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="3" t="s">
         <v>384</v>
       </c>
     </row>
@@ -4307,15 +4313,15 @@
       <c r="A203" t="s">
         <v>385</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
         <v>387</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="3" t="s">
         <v>388</v>
       </c>
     </row>
@@ -4323,7 +4329,7 @@
       <c r="A205" t="s">
         <v>389</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="3" t="s">
         <v>390</v>
       </c>
     </row>
@@ -4331,7 +4337,7 @@
       <c r="A206" t="s">
         <v>391</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="3" t="s">
         <v>392</v>
       </c>
     </row>
@@ -4339,7 +4345,7 @@
       <c r="A207" t="s">
         <v>393</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="3" t="s">
         <v>394</v>
       </c>
     </row>
@@ -4347,7 +4353,7 @@
       <c r="A208" t="s">
         <v>395</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="3" t="s">
         <v>396</v>
       </c>
     </row>
@@ -4355,7 +4361,7 @@
       <c r="A209" t="s">
         <v>397</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="3" t="s">
         <v>398</v>
       </c>
     </row>
@@ -4363,7 +4369,7 @@
       <c r="A210" t="s">
         <v>399</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="3" t="s">
         <v>400</v>
       </c>
     </row>
@@ -4371,15 +4377,15 @@
       <c r="A211" t="s">
         <v>401</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="3" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
         <v>403</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="3" t="s">
         <v>404</v>
       </c>
     </row>
@@ -4387,7 +4393,7 @@
       <c r="A213" t="s">
         <v>405</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="3" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4395,7 +4401,7 @@
       <c r="A214" t="s">
         <v>407</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="3" t="s">
         <v>408</v>
       </c>
     </row>
@@ -4403,39 +4409,39 @@
       <c r="A215" t="s">
         <v>409</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="s">
         <v>411</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="3" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="s">
         <v>413</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
         <v>415</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="s">
         <v>417</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="3" t="s">
         <v>418</v>
       </c>
     </row>
@@ -4443,7 +4449,7 @@
       <c r="A220" t="s">
         <v>419</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="3" t="s">
         <v>420</v>
       </c>
     </row>
@@ -4451,7 +4457,7 @@
       <c r="A221" t="s">
         <v>421</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="3" t="s">
         <v>422</v>
       </c>
     </row>
@@ -4459,7 +4465,7 @@
       <c r="A222" t="s">
         <v>423</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4467,7 +4473,7 @@
       <c r="A223" t="s">
         <v>424</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B223" s="3" t="s">
         <v>425</v>
       </c>
     </row>
@@ -4475,7 +4481,7 @@
       <c r="A224" t="s">
         <v>426</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4483,7 +4489,7 @@
       <c r="A225" t="s">
         <v>427</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="3" t="s">
         <v>428</v>
       </c>
     </row>
@@ -4491,7 +4497,7 @@
       <c r="A226" t="s">
         <v>429</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B226" s="3" t="s">
         <v>430</v>
       </c>
     </row>
@@ -4499,7 +4505,7 @@
       <c r="A227" t="s">
         <v>431</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B227" s="3" t="s">
         <v>432</v>
       </c>
     </row>
@@ -4507,7 +4513,7 @@
       <c r="A228" t="s">
         <v>433</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B228" s="3" t="s">
         <v>434</v>
       </c>
     </row>
@@ -4515,7 +4521,7 @@
       <c r="A229" t="s">
         <v>435</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B229" s="3" t="s">
         <v>436</v>
       </c>
     </row>
@@ -4523,15 +4529,15 @@
       <c r="A230" t="s">
         <v>437</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>439</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B231" s="3" t="s">
         <v>440</v>
       </c>
     </row>
@@ -4539,7 +4545,7 @@
       <c r="A232" t="s">
         <v>441</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="3" t="s">
         <v>442</v>
       </c>
     </row>
@@ -4547,7 +4553,7 @@
       <c r="A233" t="s">
         <v>443</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B233" s="3" t="s">
         <v>444</v>
       </c>
     </row>
@@ -4555,7 +4561,7 @@
       <c r="A234" t="s">
         <v>445</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B234" s="3" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4563,7 +4569,7 @@
       <c r="A235" t="s">
         <v>446</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B235" s="3" t="s">
         <v>447</v>
       </c>
     </row>
@@ -4571,15 +4577,15 @@
       <c r="A236" t="s">
         <v>448</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B236" s="3" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" t="s">
         <v>450</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B237" s="3" t="s">
         <v>451</v>
       </c>
     </row>
@@ -4587,7 +4593,7 @@
       <c r="A238" t="s">
         <v>452</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B238" s="3" t="s">
         <v>453</v>
       </c>
     </row>
@@ -4595,7 +4601,7 @@
       <c r="A239" t="s">
         <v>454</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B239" s="3" t="s">
         <v>455</v>
       </c>
     </row>
@@ -4603,7 +4609,7 @@
       <c r="A240" t="s">
         <v>456</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B240" s="3" t="s">
         <v>457</v>
       </c>
     </row>
@@ -4611,7 +4617,7 @@
       <c r="A241" t="s">
         <v>458</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B241" s="3" t="s">
         <v>459</v>
       </c>
     </row>
@@ -4619,7 +4625,7 @@
       <c r="A242" t="s">
         <v>460</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B242" s="3" t="s">
         <v>461</v>
       </c>
     </row>
@@ -4627,7 +4633,7 @@
       <c r="A243" t="s">
         <v>462</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B243" s="3" t="s">
         <v>463</v>
       </c>
     </row>
@@ -4635,7 +4641,7 @@
       <c r="A244" t="s">
         <v>464</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B244" s="3" t="s">
         <v>465</v>
       </c>
     </row>
@@ -4643,7 +4649,7 @@
       <c r="A245" t="s">
         <v>466</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B245" s="3" t="s">
         <v>467</v>
       </c>
     </row>
@@ -4651,7 +4657,7 @@
       <c r="A246" t="s">
         <v>468</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B246" s="3" t="s">
         <v>469</v>
       </c>
     </row>
@@ -4659,7 +4665,7 @@
       <c r="A247" t="s">
         <v>470</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B247" s="3" t="s">
         <v>471</v>
       </c>
     </row>
@@ -4667,7 +4673,7 @@
       <c r="A248" t="s">
         <v>472</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B248" s="3" t="s">
         <v>473</v>
       </c>
     </row>
@@ -4675,7 +4681,7 @@
       <c r="A249" t="s">
         <v>754</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B249" s="3" t="s">
         <v>474</v>
       </c>
     </row>
@@ -4683,7 +4689,7 @@
       <c r="A250" t="s">
         <v>475</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B250" s="3" t="s">
         <v>476</v>
       </c>
     </row>
@@ -4691,7 +4697,7 @@
       <c r="A251" t="s">
         <v>477</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B251" s="3" t="s">
         <v>478</v>
       </c>
     </row>
@@ -4699,7 +4705,7 @@
       <c r="A252" t="s">
         <v>479</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B252" s="3" t="s">
         <v>480</v>
       </c>
     </row>
@@ -4707,7 +4713,7 @@
       <c r="A253" t="s">
         <v>481</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B253" s="3" t="s">
         <v>482</v>
       </c>
     </row>
@@ -4715,7 +4721,7 @@
       <c r="A254" t="s">
         <v>483</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B254" s="3" t="s">
         <v>484</v>
       </c>
     </row>
@@ -4723,7 +4729,7 @@
       <c r="A255" t="s">
         <v>485</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B255" s="3" t="s">
         <v>486</v>
       </c>
     </row>
@@ -4731,7 +4737,7 @@
       <c r="A256" t="s">
         <v>487</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B256" s="3" t="s">
         <v>488</v>
       </c>
     </row>
@@ -4739,7 +4745,7 @@
       <c r="A257" t="s">
         <v>489</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B257" s="3" t="s">
         <v>490</v>
       </c>
     </row>
@@ -4747,7 +4753,7 @@
       <c r="A258" t="s">
         <v>491</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B258" s="3" t="s">
         <v>492</v>
       </c>
     </row>
@@ -4755,7 +4761,7 @@
       <c r="A259" t="s">
         <v>493</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B259" s="3" t="s">
         <v>494</v>
       </c>
     </row>
@@ -4763,7 +4769,7 @@
       <c r="A260" t="s">
         <v>750</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B260" s="3" t="s">
         <v>495</v>
       </c>
     </row>
@@ -4771,7 +4777,7 @@
       <c r="A261" t="s">
         <v>496</v>
       </c>
-      <c r="B261" t="s">
+      <c r="B261" s="3" t="s">
         <v>497</v>
       </c>
     </row>
@@ -4779,7 +4785,7 @@
       <c r="A262" t="s">
         <v>498</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B262" s="3" t="s">
         <v>499</v>
       </c>
     </row>
@@ -4787,7 +4793,7 @@
       <c r="A263" t="s">
         <v>500</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B263" s="3" t="s">
         <v>501</v>
       </c>
     </row>
@@ -4795,7 +4801,7 @@
       <c r="A264" t="s">
         <v>502</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B264" s="3" t="s">
         <v>503</v>
       </c>
     </row>
@@ -4803,7 +4809,7 @@
       <c r="A265" t="s">
         <v>504</v>
       </c>
-      <c r="B265" t="s">
+      <c r="B265" s="3" t="s">
         <v>505</v>
       </c>
     </row>
@@ -4811,7 +4817,7 @@
       <c r="A266" t="s">
         <v>506</v>
       </c>
-      <c r="B266" t="s">
+      <c r="B266" s="3" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4819,7 +4825,7 @@
       <c r="A267" t="s">
         <v>508</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B267" s="3" t="s">
         <v>509</v>
       </c>
     </row>
@@ -4827,7 +4833,7 @@
       <c r="A268" t="s">
         <v>510</v>
       </c>
-      <c r="B268" t="s">
+      <c r="B268" s="3" t="s">
         <v>511</v>
       </c>
     </row>
@@ -4835,7 +4841,7 @@
       <c r="A269" t="s">
         <v>512</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B269" s="3" t="s">
         <v>513</v>
       </c>
     </row>
@@ -4843,7 +4849,7 @@
       <c r="A270" t="s">
         <v>514</v>
       </c>
-      <c r="B270" t="s">
+      <c r="B270" s="3" t="s">
         <v>515</v>
       </c>
     </row>
@@ -4851,7 +4857,7 @@
       <c r="A271" t="s">
         <v>516</v>
       </c>
-      <c r="B271" t="s">
+      <c r="B271" s="3" t="s">
         <v>517</v>
       </c>
     </row>
@@ -4859,7 +4865,7 @@
       <c r="A272" t="s">
         <v>518</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B272" s="3" t="s">
         <v>519</v>
       </c>
     </row>
@@ -4867,7 +4873,7 @@
       <c r="A273" t="s">
         <v>751</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B273" s="3" t="s">
         <v>520</v>
       </c>
     </row>
@@ -4880,7 +4886,7 @@
       <c r="A275" t="s">
         <v>522</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B275" s="3" t="s">
         <v>523</v>
       </c>
     </row>
@@ -4888,7 +4894,7 @@
       <c r="A276" t="s">
         <v>524</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B276" s="3" t="s">
         <v>525</v>
       </c>
     </row>
@@ -4896,7 +4902,7 @@
       <c r="A277" t="s">
         <v>526</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B277" s="3" t="s">
         <v>527</v>
       </c>
     </row>
@@ -4904,7 +4910,7 @@
       <c r="A278" t="s">
         <v>528</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B278" s="3" t="s">
         <v>529</v>
       </c>
     </row>
@@ -4912,7 +4918,7 @@
       <c r="A279" t="s">
         <v>530</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B279" s="3" t="s">
         <v>531</v>
       </c>
     </row>
@@ -4920,15 +4926,15 @@
       <c r="A280" t="s">
         <v>532</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B280" s="3" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="s">
         <v>534</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B281" s="3" t="s">
         <v>535</v>
       </c>
     </row>
@@ -4936,15 +4942,15 @@
       <c r="A282" t="s">
         <v>536</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B282" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" t="s">
         <v>537</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B283" s="3" t="s">
         <v>538</v>
       </c>
     </row>
@@ -4952,15 +4958,15 @@
       <c r="A284" t="s">
         <v>539</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B284" s="3" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="s">
         <v>541</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B285" s="3" t="s">
         <v>542</v>
       </c>
     </row>
@@ -4968,7 +4974,7 @@
       <c r="A286" t="s">
         <v>543</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B286" s="3" t="s">
         <v>544</v>
       </c>
     </row>
@@ -4976,15 +4982,15 @@
       <c r="A287" t="s">
         <v>545</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B287" s="3" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="s">
         <v>547</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B288" s="3" t="s">
         <v>548</v>
       </c>
     </row>
@@ -4997,7 +5003,7 @@
       <c r="A290" t="s">
         <v>550</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B290" s="3" t="s">
         <v>551</v>
       </c>
     </row>
@@ -5005,7 +5011,7 @@
       <c r="A291" t="s">
         <v>552</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B291" s="3" t="s">
         <v>553</v>
       </c>
     </row>
@@ -5013,7 +5019,7 @@
       <c r="A292" t="s">
         <v>554</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B292" s="3" t="s">
         <v>555</v>
       </c>
     </row>
@@ -5021,7 +5027,7 @@
       <c r="A293" t="s">
         <v>556</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B293" s="3" t="s">
         <v>557</v>
       </c>
     </row>
@@ -5029,7 +5035,7 @@
       <c r="A294" t="s">
         <v>558</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B294" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5037,7 +5043,7 @@
       <c r="A295" t="s">
         <v>559</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B295" s="3" t="s">
         <v>560</v>
       </c>
     </row>
@@ -5050,7 +5056,7 @@
       <c r="A297" t="s">
         <v>562</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B297" s="3" t="s">
         <v>563</v>
       </c>
     </row>
@@ -5058,7 +5064,7 @@
       <c r="A298" t="s">
         <v>564</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B298" s="3" t="s">
         <v>565</v>
       </c>
     </row>
@@ -5066,7 +5072,7 @@
       <c r="A299" t="s">
         <v>566</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B299" s="3" t="s">
         <v>567</v>
       </c>
     </row>
@@ -5074,23 +5080,23 @@
       <c r="A300" t="s">
         <v>568</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B300" s="3" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>570</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B301" s="3" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
         <v>572</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B302" s="3" t="s">
         <v>573</v>
       </c>
     </row>
@@ -5098,15 +5104,15 @@
       <c r="A303" t="s">
         <v>574</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B303" s="3" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>576</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B304" s="3" t="s">
         <v>577</v>
       </c>
     </row>
@@ -5114,7 +5120,7 @@
       <c r="A305" t="s">
         <v>578</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B305" s="3" t="s">
         <v>579</v>
       </c>
     </row>
@@ -5122,7 +5128,7 @@
       <c r="A306" t="s">
         <v>580</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B306" s="3" t="s">
         <v>581</v>
       </c>
     </row>
@@ -5130,7 +5136,7 @@
       <c r="A307" t="s">
         <v>582</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B307" s="3" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5138,7 +5144,7 @@
       <c r="A308" t="s">
         <v>584</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B308" s="3" t="s">
         <v>585</v>
       </c>
     </row>
@@ -5146,15 +5152,15 @@
       <c r="A309" t="s">
         <v>586</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B309" s="3" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>588</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B310" s="3" t="s">
         <v>589</v>
       </c>
     </row>
@@ -5162,7 +5168,7 @@
       <c r="A311" t="s">
         <v>590</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B311" s="3" t="s">
         <v>591</v>
       </c>
     </row>
@@ -5170,23 +5176,23 @@
       <c r="A312" t="s">
         <v>592</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B312" s="3" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="s">
         <v>594</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B313" s="3" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="s">
         <v>596</v>
       </c>
-      <c r="B314" t="s">
+      <c r="B314" s="3" t="s">
         <v>595</v>
       </c>
     </row>
@@ -5194,7 +5200,7 @@
       <c r="A315" t="s">
         <v>597</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B315" s="3" t="s">
         <v>598</v>
       </c>
     </row>
@@ -5202,7 +5208,7 @@
       <c r="A316" t="s">
         <v>599</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B316" s="3" t="s">
         <v>179</v>
       </c>
     </row>
@@ -5210,7 +5216,7 @@
       <c r="A317" t="s">
         <v>600</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B317" s="3" t="s">
         <v>601</v>
       </c>
     </row>
@@ -5218,15 +5224,15 @@
       <c r="A318" t="s">
         <v>602</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B318" s="3" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>604</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B319" s="3" t="s">
         <v>605</v>
       </c>
     </row>
@@ -5234,7 +5240,7 @@
       <c r="A320" t="s">
         <v>606</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B320" s="3" t="s">
         <v>607</v>
       </c>
     </row>
@@ -5242,7 +5248,7 @@
       <c r="A321" t="s">
         <v>608</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B321" s="3" t="s">
         <v>609</v>
       </c>
     </row>
@@ -5250,7 +5256,7 @@
       <c r="A322" t="s">
         <v>610</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B322" s="3" t="s">
         <v>611</v>
       </c>
     </row>
@@ -5258,7 +5264,7 @@
       <c r="A323" t="s">
         <v>612</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B323" s="3" t="s">
         <v>613</v>
       </c>
     </row>
@@ -5266,7 +5272,7 @@
       <c r="A324" t="s">
         <v>614</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B324" s="3" t="s">
         <v>615</v>
       </c>
     </row>
@@ -5274,7 +5280,7 @@
       <c r="A325" t="s">
         <v>616</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B325" s="3" t="s">
         <v>617</v>
       </c>
     </row>
@@ -5282,7 +5288,7 @@
       <c r="A326" t="s">
         <v>618</v>
       </c>
-      <c r="B326" t="s">
+      <c r="B326" s="3" t="s">
         <v>619</v>
       </c>
     </row>
@@ -5290,23 +5296,23 @@
       <c r="A327" t="s">
         <v>620</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B327" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>621</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B328" s="3" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>623</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B329" s="3" t="s">
         <v>624</v>
       </c>
     </row>
@@ -5314,7 +5320,7 @@
       <c r="A330" t="s">
         <v>625</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B330" s="3" t="s">
         <v>626</v>
       </c>
     </row>
@@ -5322,7 +5328,7 @@
       <c r="A331" t="s">
         <v>627</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B331" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5330,7 +5336,7 @@
       <c r="A332" t="s">
         <v>628</v>
       </c>
-      <c r="B332" t="s">
+      <c r="B332" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5338,7 +5344,7 @@
       <c r="A333" t="s">
         <v>629</v>
       </c>
-      <c r="B333" t="s">
+      <c r="B333" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5346,7 +5352,7 @@
       <c r="A334" t="s">
         <v>630</v>
       </c>
-      <c r="B334" t="s">
+      <c r="B334" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5354,7 +5360,7 @@
       <c r="A335" t="s">
         <v>631</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B335" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5362,7 +5368,7 @@
       <c r="A336" t="s">
         <v>632</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B336" s="3" t="s">
         <v>169</v>
       </c>
     </row>
@@ -5370,7 +5376,7 @@
       <c r="A337" t="s">
         <v>633</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B337" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5378,7 +5384,7 @@
       <c r="A338" t="s">
         <v>634</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B338" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5386,15 +5392,15 @@
       <c r="A339" t="s">
         <v>635</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B339" s="3" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
         <v>637</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B340" s="3" t="s">
         <v>638</v>
       </c>
     </row>
@@ -5402,15 +5408,15 @@
       <c r="A341" t="s">
         <v>639</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B341" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>640</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B342" s="3" t="s">
         <v>641</v>
       </c>
     </row>
@@ -5418,7 +5424,7 @@
       <c r="A343" t="s">
         <v>758</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B343" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5426,7 +5432,7 @@
       <c r="A344" t="s">
         <v>642</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B344" s="3" t="s">
         <v>643</v>
       </c>
     </row>
@@ -5434,7 +5440,7 @@
       <c r="A345" t="s">
         <v>644</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B345" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5442,7 +5448,7 @@
       <c r="A346" t="s">
         <v>645</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B346" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5450,7 +5456,7 @@
       <c r="A347" t="s">
         <v>646</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B347" s="3" t="s">
         <v>647</v>
       </c>
     </row>
@@ -5458,7 +5464,7 @@
       <c r="A348" t="s">
         <v>648</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B348" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5466,7 +5472,7 @@
       <c r="A349" t="s">
         <v>649</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B349" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5474,15 +5480,15 @@
       <c r="A350" t="s">
         <v>650</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B350" s="3" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" t="s">
         <v>652</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B351" s="3" t="s">
         <v>653</v>
       </c>
     </row>
@@ -5490,7 +5496,7 @@
       <c r="A352" t="s">
         <v>654</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B352" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5498,7 +5504,7 @@
       <c r="A353" t="s">
         <v>655</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B353" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5506,7 +5512,7 @@
       <c r="A354" t="s">
         <v>656</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B354" s="3" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5514,15 +5520,15 @@
       <c r="A355" t="s">
         <v>657</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B355" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>749</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B356" s="3" t="s">
         <v>658</v>
       </c>
     </row>
@@ -5530,7 +5536,7 @@
       <c r="A357" t="s">
         <v>659</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B357" s="3" t="s">
         <v>660</v>
       </c>
     </row>
@@ -5538,7 +5544,7 @@
       <c r="A358" t="s">
         <v>661</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B358" s="3" t="s">
         <v>662</v>
       </c>
     </row>
@@ -5546,7 +5552,7 @@
       <c r="A359" t="s">
         <v>663</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B359" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5554,7 +5560,7 @@
       <c r="A360" t="s">
         <v>664</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B360" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -5562,15 +5568,15 @@
       <c r="A361" t="s">
         <v>665</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B361" s="3" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" t="s">
         <v>667</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B362" s="3" t="s">
         <v>668</v>
       </c>
     </row>
@@ -5578,7 +5584,7 @@
       <c r="A363" t="s">
         <v>669</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B363" s="3" t="s">
         <v>670</v>
       </c>
     </row>
@@ -5586,7 +5592,7 @@
       <c r="A364" t="s">
         <v>671</v>
       </c>
-      <c r="B364" t="s">
+      <c r="B364" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5594,7 +5600,7 @@
       <c r="A365" t="s">
         <v>672</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B365" s="3" t="s">
         <v>673</v>
       </c>
     </row>
@@ -5602,15 +5608,15 @@
       <c r="A366" t="s">
         <v>674</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B366" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" t="s">
         <v>675</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B367" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5618,7 +5624,7 @@
       <c r="A368" t="s">
         <v>676</v>
       </c>
-      <c r="B368" t="s">
+      <c r="B368" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5626,7 +5632,7 @@
       <c r="A369" t="s">
         <v>677</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B369" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5634,7 +5640,7 @@
       <c r="A370" t="s">
         <v>678</v>
       </c>
-      <c r="B370" t="s">
+      <c r="B370" s="3" t="s">
         <v>679</v>
       </c>
     </row>
@@ -5647,7 +5653,7 @@
       <c r="A372" t="s">
         <v>680</v>
       </c>
-      <c r="B372" t="s">
+      <c r="B372" s="3" t="s">
         <v>681</v>
       </c>
     </row>
@@ -5655,7 +5661,7 @@
       <c r="A373" t="s">
         <v>682</v>
       </c>
-      <c r="B373" t="s">
+      <c r="B373" s="3" t="s">
         <v>683</v>
       </c>
     </row>
@@ -5663,7 +5669,7 @@
       <c r="A374" t="s">
         <v>684</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B374" s="3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -5671,7 +5677,7 @@
       <c r="A375" t="s">
         <v>685</v>
       </c>
-      <c r="B375" t="s">
+      <c r="B375" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5679,7 +5685,7 @@
       <c r="A376" t="s">
         <v>686</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B376" s="3" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5687,7 +5693,7 @@
       <c r="A377" t="s">
         <v>687</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B377" s="3" t="s">
         <v>73</v>
       </c>
     </row>
@@ -5695,7 +5701,7 @@
       <c r="A378" t="s">
         <v>688</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B378" s="3" t="s">
         <v>78</v>
       </c>
     </row>
@@ -5703,7 +5709,7 @@
       <c r="A379" t="s">
         <v>689</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B379" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5711,7 +5717,7 @@
       <c r="A380" t="s">
         <v>690</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B380" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5719,7 +5725,7 @@
       <c r="A381" t="s">
         <v>691</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B381" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5727,15 +5733,15 @@
       <c r="A382" t="s">
         <v>692</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B382" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" t="s">
         <v>693</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B383" s="3" t="s">
         <v>694</v>
       </c>
     </row>
@@ -5743,23 +5749,23 @@
       <c r="A384" t="s">
         <v>695</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B384" s="3" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" t="s">
         <v>696</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B385" s="3" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" t="s">
         <v>698</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B386" s="3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5767,15 +5773,15 @@
       <c r="A387" t="s">
         <v>699</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B387" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" t="s">
         <v>748</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B388" s="3" t="s">
         <v>700</v>
       </c>
     </row>
@@ -5783,7 +5789,7 @@
       <c r="A389" t="s">
         <v>701</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B389" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5791,7 +5797,7 @@
       <c r="A390" t="s">
         <v>702</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B390" s="3" t="s">
         <v>703</v>
       </c>
     </row>
@@ -5799,7 +5805,7 @@
       <c r="A391" t="s">
         <v>704</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B391" s="3" t="s">
         <v>705</v>
       </c>
     </row>
@@ -5807,7 +5813,7 @@
       <c r="A392" t="s">
         <v>706</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B392" s="3" t="s">
         <v>707</v>
       </c>
     </row>
@@ -5815,7 +5821,7 @@
       <c r="A393" t="s">
         <v>708</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B393" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -5823,7 +5829,7 @@
       <c r="A394" t="s">
         <v>709</v>
       </c>
-      <c r="B394" t="s">
+      <c r="B394" s="3" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5831,7 +5837,7 @@
       <c r="A395" t="s">
         <v>710</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B395" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5839,7 +5845,7 @@
       <c r="A396" t="s">
         <v>711</v>
       </c>
-      <c r="B396" t="s">
+      <c r="B396" s="3" t="s">
         <v>712</v>
       </c>
     </row>
@@ -5847,15 +5853,15 @@
       <c r="A397" t="s">
         <v>713</v>
       </c>
-      <c r="B397" t="s">
+      <c r="B397" s="3" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" t="s">
         <v>715</v>
       </c>
-      <c r="B398" t="s">
+      <c r="B398" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5863,15 +5869,15 @@
       <c r="A399" t="s">
         <v>716</v>
       </c>
-      <c r="B399" t="s">
+      <c r="B399" s="3" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" t="s">
         <v>718</v>
       </c>
-      <c r="B400" t="s">
+      <c r="B400" s="3" t="s">
         <v>719</v>
       </c>
     </row>
@@ -5879,15 +5885,15 @@
       <c r="A401" t="s">
         <v>720</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B401" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" t="s">
         <v>721</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B402" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -5895,15 +5901,15 @@
       <c r="A403" t="s">
         <v>722</v>
       </c>
-      <c r="B403" t="s">
+      <c r="B403" s="3" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A404" t="s">
         <v>724</v>
       </c>
-      <c r="B404" t="s">
+      <c r="B404" s="3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -5911,7 +5917,7 @@
       <c r="A405" t="s">
         <v>725</v>
       </c>
-      <c r="B405" t="s">
+      <c r="B405" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5919,7 +5925,7 @@
       <c r="A406" t="s">
         <v>726</v>
       </c>
-      <c r="B406" t="s">
+      <c r="B406" s="3" t="s">
         <v>117</v>
       </c>
     </row>
@@ -5927,23 +5933,23 @@
       <c r="A407" t="s">
         <v>727</v>
       </c>
-      <c r="B407" t="s">
+      <c r="B407" s="3" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A408" t="s">
         <v>729</v>
       </c>
-      <c r="B408" t="s">
+      <c r="B408" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A409" t="s">
         <v>730</v>
       </c>
-      <c r="B409" t="s">
+      <c r="B409" s="3" t="s">
         <v>731</v>
       </c>
     </row>
@@ -5951,7 +5957,7 @@
       <c r="A410" t="s">
         <v>732</v>
       </c>
-      <c r="B410" t="s">
+      <c r="B410" s="3" t="s">
         <v>121</v>
       </c>
     </row>
@@ -5959,7 +5965,7 @@
       <c r="A411" t="s">
         <v>733</v>
       </c>
-      <c r="B411" t="s">
+      <c r="B411" s="3" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5967,7 +5973,7 @@
       <c r="A412" t="s">
         <v>734</v>
       </c>
-      <c r="B412" t="s">
+      <c r="B412" s="3" t="s">
         <v>735</v>
       </c>
     </row>
@@ -5975,7 +5981,7 @@
       <c r="A413" t="s">
         <v>759</v>
       </c>
-      <c r="B413" t="s">
+      <c r="B413" s="3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -5983,7 +5989,7 @@
       <c r="A414" t="s">
         <v>736</v>
       </c>
-      <c r="B414" t="s">
+      <c r="B414" s="3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -5991,7 +5997,7 @@
       <c r="A415" t="s">
         <v>737</v>
       </c>
-      <c r="B415" t="s">
+      <c r="B415" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -5999,7 +6005,7 @@
       <c r="A416" t="s">
         <v>738</v>
       </c>
-      <c r="B416" t="s">
+      <c r="B416" s="3" t="s">
         <v>739</v>
       </c>
     </row>
@@ -6007,7 +6013,7 @@
       <c r="A417" t="s">
         <v>740</v>
       </c>
-      <c r="B417" t="s">
+      <c r="B417" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -6015,7 +6021,7 @@
       <c r="A418" t="s">
         <v>741</v>
       </c>
-      <c r="B418" t="s">
+      <c r="B418" s="3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6023,7 +6029,7 @@
       <c r="A419" t="s">
         <v>742</v>
       </c>
-      <c r="B419" t="s">
+      <c r="B419" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6031,7 +6037,7 @@
       <c r="A420" t="s">
         <v>743</v>
       </c>
-      <c r="B420" t="s">
+      <c r="B420" s="3" t="s">
         <v>744</v>
       </c>
     </row>

</xml_diff>